<commit_message>
added test cases, test scenarios and confreader
</commit_message>
<xml_diff>
--- a/excel/test_scenarios.xlsx
+++ b/excel/test_scenarios.xlsx
@@ -8,15 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AZ\edureka_pom_automation\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F12EA300-83A0-4952-8114-588471B97047}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04BE94E3-A08E-4693-A2A3-1CE945E61F9A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{593A2C51-7F2B-432B-B81B-9F914E97F10A}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{593A2C51-7F2B-432B-B81B-9F914E97F10A}"/>
   </bookViews>
   <sheets>
     <sheet name="registration test scenarios" sheetId="1" r:id="rId1"/>
     <sheet name="login test scenarios" sheetId="2" r:id="rId2"/>
-    <sheet name="registration test cases" sheetId="3" r:id="rId3"/>
-    <sheet name="login test cases" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -28,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="60">
   <si>
     <t>registration test scenarios</t>
   </si>
@@ -57,9 +55,6 @@
     <t>9a</t>
   </si>
   <si>
-    <t>try to register with valid email,  valid phone number, check privacy policy box and enter valid password (8 characters)</t>
-  </si>
-  <si>
     <t>try to register with valid email ,  no phone number, checked privacy policy box</t>
   </si>
   <si>
@@ -123,21 +118,9 @@
     <t>try to log in with invalid email,  valid password</t>
   </si>
   <si>
-    <t>try to log in with invalid email,  invalid password (letters)</t>
-  </si>
-  <si>
-    <t>try to log in with valid email,  invalid password (letters)</t>
-  </si>
-  <si>
     <t>login test_scenarios</t>
   </si>
   <si>
-    <t>try to log in with valid email ,  2 character password</t>
-  </si>
-  <si>
-    <t>try to log in with valid email ,  very long password (40 characters)</t>
-  </si>
-  <si>
     <t>10a</t>
   </si>
   <si>
@@ -163,6 +146,66 @@
   </si>
   <si>
     <t>try to register with empty spaces email , empty spaces phone number, unchecked privacy policy box</t>
+  </si>
+  <si>
+    <t>try to register with valid email,  valid phone number, check privacy policy box and enter valid password (8 characters, at least 1 uppercase and at least 1 lowercase letters)</t>
+  </si>
+  <si>
+    <t>try to register with valid email,  valid phone number, check privacy policy box and enter invalid password (8 characters,all uppercase letters)</t>
+  </si>
+  <si>
+    <t>try to register with valid email,  valid phone number, check privacy policy box and enter invalid password (8 characters,all lowercase letters)</t>
+  </si>
+  <si>
+    <t>try to register with valid email,  valid phone number, check privacy policy box and enter invalid password (8 characters,all numbers)</t>
+  </si>
+  <si>
+    <t>try to register with valid email,  valid phone number, check privacy policy box and enter invalid password (2 characters, upper and lower case)</t>
+  </si>
+  <si>
+    <t>try to register with valid email,  valid phone number, check privacy policy box and enter invalid password (empty field)</t>
+  </si>
+  <si>
+    <t>try to register with valid email,  valid phone number, check privacy policy box and enter invalid password (8 blank spaces)</t>
+  </si>
+  <si>
+    <t>try to register with valid email,  valid phone number, check privacy policy box and enter invalid password (8symbols)</t>
+  </si>
+  <si>
+    <t>1a</t>
+  </si>
+  <si>
+    <t>1b</t>
+  </si>
+  <si>
+    <t>1c</t>
+  </si>
+  <si>
+    <t>1d</t>
+  </si>
+  <si>
+    <t>1e</t>
+  </si>
+  <si>
+    <t>1f</t>
+  </si>
+  <si>
+    <t>1g</t>
+  </si>
+  <si>
+    <t>1h</t>
+  </si>
+  <si>
+    <t>try to register with valid email,  valid phone number, check privacy policy box and enter valid password (51 character, at least 1 uppercase and at least 1 lowercase letters)</t>
+  </si>
+  <si>
+    <t>try to log in with invalid email,  invalid password</t>
+  </si>
+  <si>
+    <t>try to log in with valid email, wrong password</t>
+  </si>
+  <si>
+    <t>try to log in with wrong email,  invalid password</t>
   </si>
 </sst>
 </file>
@@ -207,10 +250,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -527,10 +573,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D1B5EFD-506A-4221-9B18-BFE452B69362}">
-  <dimension ref="A1:B25"/>
+  <dimension ref="A1:B33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M26" sqref="M26"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -548,183 +594,247 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>9</v>
+        <v>40</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="2">
-        <v>2</v>
+      <c r="A4" s="2" t="s">
+        <v>48</v>
       </c>
       <c r="B4" t="s">
-        <v>10</v>
+        <v>56</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>1</v>
+        <v>49</v>
       </c>
       <c r="B5" t="s">
-        <v>11</v>
+        <v>41</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="2">
-        <v>3</v>
+      <c r="A6" s="2" t="s">
+        <v>50</v>
       </c>
       <c r="B6" t="s">
-        <v>12</v>
+        <v>42</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>2</v>
+        <v>51</v>
       </c>
       <c r="B7" t="s">
-        <v>13</v>
+        <v>43</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="2">
-        <v>4</v>
+      <c r="A8" s="2" t="s">
+        <v>52</v>
       </c>
       <c r="B8" t="s">
-        <v>14</v>
+        <v>44</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>3</v>
+        <v>53</v>
       </c>
       <c r="B9" t="s">
-        <v>15</v>
+        <v>45</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="2">
-        <v>5</v>
+      <c r="A10" s="2" t="s">
+        <v>54</v>
       </c>
       <c r="B10" t="s">
-        <v>16</v>
+        <v>46</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>4</v>
+        <v>55</v>
       </c>
       <c r="B11" t="s">
-        <v>21</v>
+        <v>47</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="B12" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="B13" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="B14" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="B15" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B16" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="B17" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B18" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B19" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="B20" t="s">
-        <v>37</v>
+        <v>16</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
-        <v>36</v>
+        <v>5</v>
       </c>
       <c r="B21" t="s">
-        <v>38</v>
+        <v>21</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="B22" t="s">
-        <v>41</v>
+        <v>17</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
-        <v>39</v>
+        <v>6</v>
       </c>
       <c r="B23" t="s">
-        <v>42</v>
+        <v>22</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="2">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B24" t="s">
-        <v>43</v>
+        <v>18</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
-        <v>40</v>
+        <v>7</v>
       </c>
       <c r="B25" t="s">
-        <v>44</v>
+        <v>23</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" s="2">
+        <v>9</v>
+      </c>
+      <c r="B26" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B27" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" s="2">
+        <v>10</v>
+      </c>
+      <c r="B28" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B29" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" s="2">
+        <v>11</v>
+      </c>
+      <c r="B30" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B31" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" s="2">
+        <v>12</v>
+      </c>
+      <c r="B32" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B33" t="s">
+        <v>39</v>
       </c>
     </row>
   </sheetData>
@@ -735,17 +845,17 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5ACB75C5-7B56-46A0-989A-A4D9A6EDF575}">
-  <dimension ref="A1:B11"/>
+  <dimension ref="A1:B10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -753,7 +863,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -761,7 +871,7 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -769,7 +879,7 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -777,7 +887,7 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -785,7 +895,7 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -793,7 +903,7 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>30</v>
+        <v>59</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -801,52 +911,18 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>31</v>
+        <v>58</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="2">
+      <c r="A10" s="3">
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" s="2">
-        <v>9</v>
-      </c>
-      <c r="B11" t="s">
-        <v>35</v>
+        <v>57</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A3D2329-C8BF-434F-BE4A-E6298FD26B9C}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J32" sqref="J32"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{64B65011-A486-4F66-A82A-410835281E93}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>